<commit_message>
chore: updated sprint-02 planning doc and feature board
Signed-off-by: Levin Schulze <levin.f.schulze@campus.tu-berlin.de>
</commit_message>
<xml_diff>
--- a/Deliverables/sprint-02/planning-document.xlsx
+++ b/Deliverables/sprint-02/planning-document.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="210">
   <si>
     <t>Project Name</t>
   </si>
@@ -77,17 +77,16 @@
     <t>Additional materials</t>
   </si>
   <si>
-    <r>
-      <rPr/>
-      <t xml:space="preserve">Discord: </t>
-    </r>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>https://discord.gg/mhFBrsTx</t>
-    </r>
+    <t>Discord</t>
+  </si>
+  <si>
+    <t>https://discord.gg/mhFBrsTx</t>
+  </si>
+  <si>
+    <t>Figma Link Website</t>
+  </si>
+  <si>
+    <t>https://www.figma.com/design/kLihICBMvBVKCodv1OlY4Y/Website-Design?m=auto&amp;t=UItPz3hhwCtSgsc5-1</t>
   </si>
   <si>
     <t>Team maling list</t>
@@ -186,7 +185,7 @@
     <t>HansKiller-TH</t>
   </si>
   <si>
-    <t>hans.killer@fau.de</t>
+    <t>hanskiller@web.de</t>
   </si>
   <si>
     <t>Schulze</t>
@@ -249,10 +248,10 @@
     <t>Hans Killer</t>
   </si>
   <si>
+    <t>Build Process Review</t>
+  </si>
+  <si>
     <t>Robin Rose Raju</t>
-  </si>
-  <si>
-    <t>Build Process Review</t>
   </si>
   <si>
     <t>Ervin Nogu</t>
@@ -552,6 +551,99 @@
   </si>
   <si>
     <t>Component library built on Tailwind CSS.</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>20.3.7</t>
+  </si>
+  <si>
+    <t>typescript</t>
+  </si>
+  <si>
+    <t>5.9.3</t>
+  </si>
+  <si>
+    <t>Apache-2.0</t>
+  </si>
+  <si>
+    <t>zonejs</t>
+  </si>
+  <si>
+    <t>0.15.1</t>
+  </si>
+  <si>
+    <t>tslib</t>
+  </si>
+  <si>
+    <t>2.8.1</t>
+  </si>
+  <si>
+    <t>karma</t>
+  </si>
+  <si>
+    <t>6.4.4</t>
+  </si>
+  <si>
+    <t>karma-chrome-launcher</t>
+  </si>
+  <si>
+    <t>3.2.0</t>
+  </si>
+  <si>
+    <t>karma-coverage</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>karma-jasmine</t>
+  </si>
+  <si>
+    <t>5.1.0</t>
+  </si>
+  <si>
+    <t>karma-jasmine-html-reporter</t>
+  </si>
+  <si>
+    <t>2.1.0</t>
+  </si>
+  <si>
+    <t>postcss</t>
+  </si>
+  <si>
+    <t>8.5.6</t>
+  </si>
+  <si>
+    <t>rxjs</t>
+  </si>
+  <si>
+    <t>7.8.2</t>
+  </si>
+  <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>2.3.232</t>
+  </si>
+  <si>
+    <t>MLP 2.0</t>
+  </si>
+  <si>
+    <t>spring-boot</t>
+  </si>
+  <si>
+    <t>3.5.6</t>
+  </si>
+  <si>
+    <t>Derived from Githubs SBOM (direct relationship)</t>
+  </si>
+  <si>
+    <t>Starting next week will use an SBOM Tool (Syft/trivy) and will be updated in Github Deliveries</t>
   </si>
   <si>
     <t>Value</t>
@@ -598,7 +690,7 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -608,6 +700,10 @@
       <b/>
     </font>
     <font/>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
     <font>
       <u/>
       <color rgb="FF0000FF"/>
@@ -689,7 +785,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="108">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -711,6 +807,18 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
@@ -750,9 +858,6 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
@@ -771,30 +876,30 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -807,7 +912,7 @@
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -825,166 +930,166 @@
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="8" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="8" fontId="9" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1432,29 +1537,31 @@
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1"/>
-      <c r="B18" s="3"/>
+      <c r="B17" s="10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="1"/>
-      <c r="B19" s="3"/>
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1"/>
@@ -1466,14 +1573,15 @@
     <hyperlink r:id="rId2" ref="B8"/>
     <hyperlink r:id="rId3" ref="B9"/>
     <hyperlink r:id="rId4" ref="B10"/>
-    <hyperlink r:id="rId5" ref="B15"/>
+    <hyperlink r:id="rId5" ref="B16"/>
+    <hyperlink r:id="rId6" ref="B17"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1497,405 +1605,405 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="74" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="48" t="s">
+      <c r="A1" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="B1" s="77" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="D1" s="51" t="s">
         <v>140</v>
       </c>
+      <c r="E1" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="49"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3">
-      <c r="A3" s="51" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
+      <c r="A3" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
     </row>
     <row r="4">
-      <c r="A4" s="49"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
     </row>
     <row r="5">
-      <c r="A5" s="54" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="56">
+      <c r="A5" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="59">
         <f>sum(D8:D13)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="56">
+      <c r="E5" s="59">
         <f>D5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6">
-      <c r="A6" s="49"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
     </row>
     <row r="7">
-      <c r="A7" s="57" t="s">
-        <v>143</v>
-      </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
+      <c r="A7" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="78"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
     </row>
     <row r="8">
-      <c r="A8" s="49"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="60" t="s">
-        <v>144</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="60" t="s">
-        <v>145</v>
+      <c r="A8" s="52"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="63" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="63" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="61">
+      <c r="A9" s="64">
         <v>1.0</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="56">
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="59">
         <f>sum(D16:D21)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="59">
         <f>$D$5</f>
         <v>0</v>
       </c>
-      <c r="F9" s="56">
+      <c r="F9" s="59">
         <f>sum(F16:F21)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="56">
+      <c r="G9" s="59">
         <f>$D$5</f>
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="49">
+      <c r="A10" s="52">
         <f t="shared" ref="A10:A11" si="1">A9+1</f>
         <v>2</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="62">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="65">
         <f>sum(D22:D27)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="62">
+      <c r="E10" s="65">
         <f t="shared" ref="E10:E12" si="2">E9-D9</f>
         <v>0</v>
       </c>
-      <c r="F10" s="62">
+      <c r="F10" s="65">
         <f>sum(F22:F27)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="62">
+      <c r="G10" s="65">
         <f t="shared" ref="G10:G12" si="3">G9-F9</f>
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="61">
+      <c r="A11" s="64">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="56">
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="59">
         <f>sum(D28:D33)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="56">
+      <c r="E11" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F11" s="56">
+      <c r="F11" s="59">
         <f>sum(F28:F33)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="56">
+      <c r="G11" s="59">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="62">
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="65">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="62">
+      <c r="F12" s="35"/>
+      <c r="G12" s="65">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="61"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14">
-      <c r="A14" s="65" t="s">
-        <v>146</v>
-      </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
+      <c r="A14" s="68" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" s="69"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
     </row>
     <row r="15">
-      <c r="A15" s="61"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
+      <c r="A15" s="64"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
     </row>
     <row r="16">
-      <c r="A16" s="68">
+      <c r="A16" s="71">
         <f>A9</f>
         <v>1</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
     </row>
     <row r="17">
-      <c r="A17" s="61"/>
-      <c r="B17" s="70"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
+      <c r="A17" s="64"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
     </row>
     <row r="18">
-      <c r="A18" s="49"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="50"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19">
-      <c r="A19" s="61"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="33"/>
+      <c r="A19" s="64"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="36"/>
     </row>
     <row r="20">
-      <c r="A20" s="72"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="64"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="67"/>
     </row>
     <row r="21">
-      <c r="A21" s="61"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="33"/>
+      <c r="A21" s="64"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22">
-      <c r="A22" s="68">
+      <c r="A22" s="71">
         <f>A10</f>
         <v>2</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
     </row>
     <row r="23">
-      <c r="A23" s="61"/>
-      <c r="B23" s="70"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24">
-      <c r="A24" s="72"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="64"/>
+      <c r="A24" s="75"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="67"/>
     </row>
     <row r="25">
-      <c r="A25" s="61"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="33"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="36"/>
     </row>
     <row r="26">
-      <c r="A26" s="72"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="64"/>
+      <c r="A26" s="75"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="67"/>
     </row>
     <row r="27">
-      <c r="A27" s="61"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="33"/>
+      <c r="A27" s="64"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28">
-      <c r="A28" s="68">
+      <c r="A28" s="71">
         <f>A11</f>
         <v>3</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
     </row>
     <row r="29">
-      <c r="A29" s="61"/>
-      <c r="B29" s="70"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
+      <c r="A29" s="64"/>
+      <c r="B29" s="73"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
     </row>
     <row r="30">
-      <c r="A30" s="72"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
+      <c r="A30" s="75"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
     </row>
     <row r="31">
-      <c r="A31" s="61"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
+      <c r="A31" s="64"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
     </row>
     <row r="32">
-      <c r="A32" s="72"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
+      <c r="A32" s="75"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
     </row>
     <row r="33">
-      <c r="A33" s="61"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="73" t="s">
-        <v>147</v>
-      </c>
-      <c r="D33" s="56"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
+      <c r="A33" s="64"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="76" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="59"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34">
-      <c r="A34" s="72"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
+      <c r="A34" s="75"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1923,17 +2031,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="76" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="D1" s="77" t="s">
-        <v>150</v>
+      <c r="A1" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="80" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="2">
@@ -2077,10 +2185,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2">
@@ -2189,23 +2297,23 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
-        <v>55</v>
+      <c r="A1" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2">
@@ -2213,19 +2321,19 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3">
@@ -2233,123 +2341,253 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="A11" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="A12" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="A13" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="A14" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="A15" s="2">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="A16" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17">
@@ -2374,7 +2612,9 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="F19" s="2" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="3"/>
@@ -2382,7 +2622,9 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="F20" s="2" t="s">
+        <v>197</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2411,314 +2653,304 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="78" t="str">
+      <c r="A1" s="81" t="str">
         <f>'Project Team'!A1</f>
         <v>Last Name</v>
       </c>
-      <c r="B1" s="78" t="str">
+      <c r="B1" s="81" t="str">
         <f>'Project Team'!B1</f>
         <v>First Name</v>
       </c>
-      <c r="C1" s="79" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
+      <c r="C1" s="82" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="83"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
     </row>
     <row r="2">
-      <c r="A2" s="84" t="str">
+      <c r="A2" s="87" t="str">
         <f>'Project Team'!A2</f>
         <v>Wysokinska</v>
       </c>
-      <c r="B2" s="84" t="str">
+      <c r="B2" s="87" t="str">
         <f>'Project Team'!B2</f>
         <v>Xemena</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="87">
+      <c r="C2" s="88"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="90" t="str">
         <f>average(C2:C10)</f>
-        <v>2.8</v>
-      </c>
-      <c r="F2" s="88" t="str">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F2" s="91" t="str">
         <f>if(stdev(C2:C7) &gt; 0,"NOK", "OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
     </row>
     <row r="3">
-      <c r="A3" s="90" t="str">
+      <c r="A3" s="93" t="str">
         <f>'Project Team'!A3</f>
         <v>Ostrizki</v>
       </c>
-      <c r="B3" s="90" t="str">
+      <c r="B3" s="93" t="str">
         <f>'Project Team'!B3</f>
         <v>Jan</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="91"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="94"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
     </row>
     <row r="4">
-      <c r="A4" s="84" t="str">
+      <c r="A4" s="87" t="str">
         <f>'Project Team'!A4</f>
         <v>Raju</v>
       </c>
-      <c r="B4" s="84" t="str">
+      <c r="B4" s="87" t="str">
         <f>'Project Team'!B4</f>
         <v>Robin Jose </v>
       </c>
-      <c r="C4" s="85">
-        <v>3.0</v>
-      </c>
-      <c r="D4" s="86"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="89"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
     </row>
     <row r="5">
-      <c r="A5" s="90" t="str">
+      <c r="A5" s="93" t="str">
         <f>'Project Team'!A5</f>
         <v>Nogu</v>
       </c>
-      <c r="B5" s="90" t="str">
+      <c r="B5" s="93" t="str">
         <f>'Project Team'!B5</f>
         <v>Ervin</v>
       </c>
-      <c r="C5" s="85">
-        <v>3.0</v>
-      </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
     </row>
     <row r="6">
-      <c r="A6" s="84" t="str">
+      <c r="A6" s="87" t="str">
         <f>'Project Team'!A6</f>
         <v>Krüger</v>
       </c>
-      <c r="B6" s="84" t="str">
+      <c r="B6" s="87" t="str">
         <f>'Project Team'!B6</f>
         <v>Landolf</v>
       </c>
-      <c r="C6" s="85">
-        <v>3.0</v>
-      </c>
-      <c r="D6" s="94"/>
-      <c r="E6" s="95">
+      <c r="C6" s="88"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="98">
         <v>0.0</v>
       </c>
-      <c r="F6" s="96" t="s">
-        <v>165</v>
-      </c>
-      <c r="G6" s="89"/>
-      <c r="H6" s="89"/>
+      <c r="F6" s="99" t="s">
+        <v>199</v>
+      </c>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
     </row>
     <row r="7">
-      <c r="A7" s="90" t="str">
+      <c r="A7" s="93" t="str">
         <f>'Project Team'!A7</f>
         <v>Tröger</v>
       </c>
-      <c r="B7" s="90" t="str">
+      <c r="B7" s="93" t="str">
         <f>'Project Team'!B7</f>
         <v>Nicolas</v>
       </c>
-      <c r="C7" s="85">
-        <v>3.0</v>
-      </c>
-      <c r="D7" s="93"/>
-      <c r="E7" s="95">
+      <c r="C7" s="88"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="98">
         <v>1.0</v>
       </c>
-      <c r="F7" s="96" t="s">
-        <v>166</v>
-      </c>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
+      <c r="F7" s="99" t="s">
+        <v>200</v>
+      </c>
+      <c r="G7" s="95"/>
+      <c r="H7" s="95"/>
     </row>
     <row r="8">
-      <c r="A8" s="84" t="str">
+      <c r="A8" s="87" t="str">
         <f t="shared" ref="A8:B8" si="1">#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="84" t="str">
+      <c r="B8" s="87" t="str">
         <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="95">
+      <c r="C8" s="100"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="98">
         <v>2.0</v>
       </c>
-      <c r="F8" s="96" t="s">
-        <v>167</v>
-      </c>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
+      <c r="F8" s="99" t="s">
+        <v>201</v>
+      </c>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
     </row>
     <row r="9">
-      <c r="A9" s="90" t="str">
+      <c r="A9" s="93" t="str">
         <f>'Project Team'!A8</f>
         <v>Killer</v>
       </c>
-      <c r="B9" s="90" t="str">
+      <c r="B9" s="93" t="str">
         <f>'Project Team'!B8</f>
         <v>Hans</v>
       </c>
-      <c r="C9" s="85">
-        <v>2.0</v>
-      </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="95">
+      <c r="C9" s="88"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="98">
         <v>3.0</v>
       </c>
-      <c r="F9" s="96" t="s">
-        <v>168</v>
-      </c>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92"/>
+      <c r="F9" s="99" t="s">
+        <v>202</v>
+      </c>
+      <c r="G9" s="95"/>
+      <c r="H9" s="95"/>
     </row>
     <row r="10">
-      <c r="A10" s="84" t="str">
+      <c r="A10" s="87" t="str">
         <f>'Project Team'!A9</f>
         <v>Schulze</v>
       </c>
-      <c r="B10" s="84" t="str">
+      <c r="B10" s="87" t="str">
         <f>'Project Team'!B9</f>
         <v>Levin</v>
       </c>
-      <c r="C10" s="85"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="95">
+      <c r="C10" s="88"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="98">
         <v>5.0</v>
       </c>
-      <c r="F10" s="96" t="s">
-        <v>169</v>
-      </c>
-      <c r="G10" s="89"/>
-      <c r="H10" s="89"/>
+      <c r="F10" s="99" t="s">
+        <v>203</v>
+      </c>
+      <c r="G10" s="92"/>
+      <c r="H10" s="92"/>
     </row>
     <row r="11">
-      <c r="A11" s="90"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="93"/>
-      <c r="E11" s="95">
+      <c r="A11" s="93"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="98">
         <v>8.0</v>
       </c>
-      <c r="F11" s="96" t="s">
-        <v>170</v>
-      </c>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
+      <c r="F11" s="99" t="s">
+        <v>204</v>
+      </c>
+      <c r="G11" s="95"/>
+      <c r="H11" s="95"/>
     </row>
     <row r="12">
-      <c r="A12" s="84"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="95">
+      <c r="A12" s="87"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="97"/>
+      <c r="E12" s="98">
         <v>13.0</v>
       </c>
-      <c r="F12" s="96" t="s">
-        <v>171</v>
-      </c>
-      <c r="G12" s="89"/>
-      <c r="H12" s="89"/>
+      <c r="F12" s="99" t="s">
+        <v>205</v>
+      </c>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
     </row>
     <row r="13">
-      <c r="A13" s="90"/>
-      <c r="B13" s="90"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="92"/>
+      <c r="A13" s="93"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="95"/>
+      <c r="H13" s="95"/>
     </row>
     <row r="14">
-      <c r="A14" s="99" t="s">
-        <v>172</v>
-      </c>
-      <c r="B14" s="100"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="100"/>
-      <c r="H14" s="100"/>
+      <c r="A14" s="102" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="103"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="103"/>
     </row>
     <row r="15">
-      <c r="A15" s="101"/>
-      <c r="B15" s="101"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="101"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="104"/>
+      <c r="G15" s="104"/>
+      <c r="H15" s="104"/>
     </row>
     <row r="16">
-      <c r="A16" s="102" t="s">
-        <v>173</v>
-      </c>
-      <c r="B16" s="103"/>
-      <c r="C16" s="103"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="103"/>
-      <c r="F16" s="103"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="103"/>
+      <c r="A16" s="105" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" s="106"/>
+      <c r="C16" s="106"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="106"/>
+      <c r="F16" s="106"/>
+      <c r="G16" s="106"/>
+      <c r="H16" s="106"/>
     </row>
     <row r="17">
-      <c r="A17" s="104" t="s">
-        <v>174</v>
-      </c>
-      <c r="B17" s="101"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="101"/>
+      <c r="A17" s="107" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" s="104"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="104"/>
     </row>
     <row r="18">
-      <c r="A18" s="102" t="s">
-        <v>175</v>
-      </c>
-      <c r="B18" s="103"/>
-      <c r="C18" s="103"/>
-      <c r="D18" s="103"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="103"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="103"/>
+      <c r="A18" s="105" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="106"/>
+      <c r="C18" s="106"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
+      <c r="F18" s="106"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="106"/>
     </row>
     <row r="19">
-      <c r="A19" s="101"/>
-      <c r="B19" s="101"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="101"/>
-      <c r="H19" s="101"/>
+      <c r="A19" s="104"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
     </row>
     <row r="20">
-      <c r="A20" s="103"/>
-      <c r="B20" s="103"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="103"/>
-      <c r="E20" s="103"/>
-      <c r="F20" s="103"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="103"/>
+      <c r="A20" s="106"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="106"/>
+      <c r="H20" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2749,186 +2981,186 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>23</v>
       </c>
+      <c r="B1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="B2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="8"/>
+      <c r="A3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="12"/>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
+      <c r="B4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="A5" s="12" t="s">
         <v>38</v>
       </c>
+      <c r="B5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="A6" s="12" t="s">
         <v>42</v>
       </c>
+      <c r="B6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="A7" s="12" t="s">
         <v>46</v>
       </c>
+      <c r="B7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="A8" s="12" t="s">
         <v>50</v>
       </c>
+      <c r="B8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="10"/>
+      <c r="A9" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="14"/>
     </row>
     <row r="11">
-      <c r="A11" s="10"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13">
-      <c r="A13" s="7"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
     </row>
     <row r="14">
-      <c r="A14" s="10"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15">
-      <c r="A15" s="10"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="17">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
     </row>
     <row r="18">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
     </row>
     <row r="19">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2959,464 +3191,464 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="12"/>
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2">
-      <c r="A2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="A2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="B2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="C2" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="D2" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="E2" s="18" t="s">
         <v>62</v>
       </c>
+      <c r="F2" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="16">
+      <c r="A3" s="20">
         <v>0.0</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="21">
         <v>45945.0</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="18" t="s">
+      <c r="C3" s="12" t="s">
         <v>66</v>
       </c>
+      <c r="D3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="16">
+      <c r="A4" s="20">
         <v>1.0</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="23">
         <f t="shared" ref="B4:B12" si="1">B3+7</f>
         <v>45952</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="F4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="21"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5">
-      <c r="A5" s="16">
+      <c r="A5" s="20">
         <v>2.0</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="23">
         <f t="shared" si="1"/>
         <v>45959</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6">
-      <c r="A6" s="16">
+      <c r="A6" s="20">
         <v>3.0</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="23">
         <f t="shared" si="1"/>
         <v>45966</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="F6" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>72</v>
+      <c r="H6" s="22" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="16">
+      <c r="A7" s="20">
         <v>4.0</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="23">
         <f t="shared" si="1"/>
         <v>45973</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H7" s="21"/>
+      <c r="H7" s="24"/>
     </row>
     <row r="8">
-      <c r="A8" s="16">
+      <c r="A8" s="20">
         <v>5.0</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="23">
         <f t="shared" si="1"/>
         <v>45980</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="F8" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" s="21"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9">
-      <c r="A9" s="16">
+      <c r="A9" s="20">
         <v>6.0</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="23">
         <f t="shared" si="1"/>
         <v>45987</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>75</v>
+      <c r="H9" s="22" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="16">
+      <c r="A10" s="20">
         <v>7.0</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="23">
         <f t="shared" si="1"/>
         <v>45994</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="F10" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="21"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11">
-      <c r="A11" s="16">
+      <c r="A11" s="20">
         <v>8.0</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="23">
         <f t="shared" si="1"/>
         <v>46001</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="21"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12">
-      <c r="A12" s="16">
+      <c r="A12" s="20">
         <v>9.0</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="23">
         <f t="shared" si="1"/>
         <v>46008</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="F12" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="21"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="13">
-      <c r="A13" s="16">
+      <c r="A13" s="20">
         <v>10.0</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="21">
         <v>46029.0</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="21"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14">
-      <c r="A14" s="16">
+      <c r="A14" s="20">
         <v>11.0</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="23">
         <f t="shared" ref="B14:B17" si="2">B13+7</f>
         <v>46036</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="F14" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="21"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15">
-      <c r="A15" s="16">
+      <c r="A15" s="20">
         <v>12.0</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="23">
         <f t="shared" si="2"/>
         <v>46043</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="21"/>
+      <c r="H15" s="24"/>
     </row>
     <row r="16">
-      <c r="A16" s="16">
+      <c r="A16" s="20">
         <v>13.0</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="23">
         <f t="shared" si="2"/>
         <v>46050</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="F16" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="18"/>
+      <c r="H16" s="22"/>
     </row>
     <row r="17">
-      <c r="A17" s="16">
+      <c r="A17" s="20">
         <v>14.0</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="23">
         <f t="shared" si="2"/>
         <v>46057</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>76</v>
+      <c r="H17" s="22" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="24"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="27"/>
     </row>
     <row r="19">
-      <c r="A19" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="24"/>
+      <c r="A19" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="27"/>
     </row>
     <row r="20">
-      <c r="A20" s="26"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="24"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="27"/>
     </row>
     <row r="21">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="24"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3447,188 +3679,188 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="28"/>
+      <c r="A1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="31"/>
     </row>
     <row r="2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30" t="s">
-        <v>79</v>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="32"/>
+      <c r="A3" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="35"/>
     </row>
     <row r="4">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30" t="s">
-        <v>81</v>
+      <c r="A4" s="32"/>
+      <c r="B4" s="33" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>82</v>
+      <c r="A5" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="29"/>
-      <c r="B6" s="30" t="s">
-        <v>83</v>
+      <c r="A6" s="32"/>
+      <c r="B6" s="33" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="32"/>
+      <c r="A7" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="35"/>
     </row>
     <row r="8">
-      <c r="A8" s="29"/>
-      <c r="B8" s="30" t="s">
-        <v>85</v>
+      <c r="A8" s="32"/>
+      <c r="B8" s="33" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" s="32"/>
+      <c r="A9" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="35"/>
     </row>
     <row r="10">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30" t="s">
-        <v>87</v>
+      <c r="A10" s="32"/>
+      <c r="B10" s="33" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="32"/>
+      <c r="A11" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="35"/>
     </row>
     <row r="12">
-      <c r="A12" s="33"/>
-      <c r="B12" s="30" t="s">
-        <v>89</v>
+      <c r="A12" s="36"/>
+      <c r="B12" s="33" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="32"/>
+      <c r="A13" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="35"/>
     </row>
     <row r="14">
-      <c r="A14" s="33"/>
-      <c r="B14" s="30" t="s">
-        <v>91</v>
+      <c r="A14" s="36"/>
+      <c r="B14" s="33" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15" s="32"/>
+      <c r="A15" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="35"/>
     </row>
     <row r="16">
-      <c r="A16" s="33"/>
-      <c r="B16" s="30" t="s">
-        <v>93</v>
+      <c r="A16" s="36"/>
+      <c r="B16" s="33" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17" s="32"/>
+      <c r="A17" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="35"/>
     </row>
     <row r="18">
-      <c r="A18" s="33"/>
-      <c r="B18" s="30" t="s">
-        <v>95</v>
+      <c r="A18" s="36"/>
+      <c r="B18" s="33" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="34"/>
+      <c r="A19" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="37"/>
     </row>
     <row r="21">
-      <c r="A21" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>65</v>
+      <c r="A21" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>68</v>
+      <c r="A22" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>67</v>
+      <c r="A23" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>99</v>
+      <c r="A24" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
     <row r="29">
-      <c r="A29" s="35" t="s">
-        <v>98</v>
+      <c r="A29" s="38" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3656,23 +3888,23 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>101</v>
+      <c r="A1" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="41"/>
     </row>
     <row r="3">
-      <c r="A3" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>102</v>
+      <c r="A3" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -3702,99 +3934,99 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>104</v>
+      <c r="A1" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13">
@@ -3852,141 +4084,141 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="41" t="s">
-        <v>127</v>
+      <c r="A1" s="44" t="s">
+        <v>130</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="42">
+      <c r="A2" s="45">
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="42">
+      <c r="A3" s="45">
         <f t="shared" ref="A3:A16" si="1">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="42">
+      <c r="A4" s="45">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="42">
+      <c r="A5" s="45">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>130</v>
+      <c r="B5" s="9" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="42">
+      <c r="A6" s="45">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="42">
+      <c r="A7" s="45">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="42">
+      <c r="A8" s="45">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9">
-      <c r="A9" s="42">
+      <c r="A9" s="45">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10">
-      <c r="A10" s="42">
+      <c r="A10" s="45">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="42">
+      <c r="A11" s="45">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12">
-      <c r="A12" s="42">
+      <c r="A12" s="45">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="42">
+      <c r="A13" s="45">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="3"/>
     </row>
     <row r="14">
-      <c r="A14" s="42">
+      <c r="A14" s="45">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15">
-      <c r="A15" s="42">
+      <c r="A15" s="45">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16">
-      <c r="A16" s="42">
+      <c r="A16" s="45">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17">
-      <c r="A17" s="42"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="3"/>
     </row>
     <row r="18">
-      <c r="A18" s="42"/>
+      <c r="A18" s="45"/>
       <c r="B18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="43"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="3"/>
     </row>
     <row r="20">
-      <c r="A20" s="43"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="3"/>
     </row>
   </sheetData>
@@ -4001,6 +4233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4015,135 +4248,138 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="41" t="s">
-        <v>127</v>
+      <c r="A1" s="44" t="s">
+        <v>130</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="42">
+      <c r="A2" s="45">
         <v>1.0</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="42">
+      <c r="A3" s="45">
         <f t="shared" ref="A3:A16" si="1">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="42">
+      <c r="A4" s="45">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="42">
+      <c r="A5" s="45">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="42">
+      <c r="A6" s="45">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="42">
+      <c r="A7" s="45">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="42">
+      <c r="A8" s="45">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9">
-      <c r="A9" s="42">
+      <c r="A9" s="45">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10">
-      <c r="A10" s="42">
+      <c r="A10" s="45">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="42">
+      <c r="A11" s="45">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12">
-      <c r="A12" s="42">
+      <c r="A12" s="45">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="42">
+      <c r="A13" s="45">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="3"/>
     </row>
     <row r="14">
-      <c r="A14" s="42">
+      <c r="A14" s="45">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15">
-      <c r="A15" s="42">
+      <c r="A15" s="45">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16">
-      <c r="A16" s="42">
+      <c r="A16" s="45">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17">
-      <c r="A17" s="42"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="3"/>
     </row>
     <row r="18">
-      <c r="A18" s="42"/>
-      <c r="B18" s="44" t="s">
-        <v>133</v>
+      <c r="A18" s="45"/>
+      <c r="B18" s="47" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="43"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="3"/>
     </row>
     <row r="20">
-      <c r="A20" s="43"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="3"/>
     </row>
   </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
@@ -4170,414 +4406,414 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="48" t="s">
+      <c r="A1" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="D1" s="51" t="s">
         <v>140</v>
       </c>
+      <c r="E1" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3">
-      <c r="A3" s="51" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
+      <c r="A3" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
     </row>
     <row r="4">
-      <c r="A4" s="49"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
     </row>
     <row r="5">
-      <c r="A5" s="54" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="56">
+      <c r="A5" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="58"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="59">
         <f>sum(D8:D13)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="56">
+      <c r="E5" s="59">
         <f>D5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6">
-      <c r="A6" s="49"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
     </row>
     <row r="7">
-      <c r="A7" s="57" t="s">
-        <v>143</v>
-      </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
+      <c r="A7" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="61"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
     </row>
     <row r="8">
-      <c r="A8" s="49"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="60" t="s">
-        <v>144</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="60" t="s">
-        <v>145</v>
+      <c r="A8" s="52"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="63" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="63" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="61">
+      <c r="A9" s="64">
         <v>1.0</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="56">
+      <c r="B9" s="57"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="59">
         <f>sum(D16:D21)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="59">
         <f>$D$5</f>
         <v>0</v>
       </c>
-      <c r="F9" s="56">
+      <c r="F9" s="59">
         <f>sum(F16:F21)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="56">
+      <c r="G9" s="59">
         <f>$D$5</f>
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="49">
+      <c r="A10" s="52">
         <f t="shared" ref="A10:A11" si="1">A9+1</f>
         <v>2</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="62">
+      <c r="B10" s="53"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="65">
         <f>sum(D22:D27)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="62">
+      <c r="E10" s="65">
         <f t="shared" ref="E10:E12" si="2">E9-D9</f>
         <v>0</v>
       </c>
-      <c r="F10" s="62">
+      <c r="F10" s="65">
         <f>sum(F22:F27)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="62">
+      <c r="G10" s="65">
         <f t="shared" ref="G10:G12" si="3">G9-F9</f>
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="61">
+      <c r="A11" s="64">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="56">
+      <c r="B11" s="57"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="59">
         <f>sum(D28:D33)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="56">
+      <c r="E11" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F11" s="56">
+      <c r="F11" s="59">
         <f>sum(F28:F33)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="56">
+      <c r="G11" s="59">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="62">
+      <c r="B12" s="67"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="65">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="62">
+      <c r="F12" s="35"/>
+      <c r="G12" s="65">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="61"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14">
-      <c r="A14" s="65" t="s">
-        <v>146</v>
-      </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
+      <c r="A14" s="68" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" s="69"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
     </row>
     <row r="15">
-      <c r="A15" s="61"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
+      <c r="A15" s="64"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
     </row>
     <row r="16">
-      <c r="A16" s="68">
+      <c r="A16" s="71">
         <f t="shared" ref="A16:B16" si="4">A9</f>
         <v>1</v>
       </c>
-      <c r="B16" s="69" t="str">
+      <c r="B16" s="72" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
     </row>
     <row r="17">
-      <c r="A17" s="61"/>
-      <c r="B17" s="70"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
+      <c r="A17" s="64"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
     </row>
     <row r="18">
-      <c r="A18" s="49"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="50"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19">
-      <c r="A19" s="61"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="33"/>
+      <c r="A19" s="64"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="36"/>
     </row>
     <row r="20">
-      <c r="A20" s="72"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="64"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="67"/>
     </row>
     <row r="21">
-      <c r="A21" s="61"/>
-      <c r="B21" s="70"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="33"/>
+      <c r="A21" s="64"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22">
-      <c r="A22" s="68">
+      <c r="A22" s="71">
         <f t="shared" ref="A22:B22" si="5">A10</f>
         <v>2</v>
       </c>
-      <c r="B22" s="69" t="str">
+      <c r="B22" s="72" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
     </row>
     <row r="23">
-      <c r="A23" s="61"/>
-      <c r="B23" s="70"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24">
-      <c r="A24" s="72"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="64"/>
+      <c r="A24" s="75"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="67"/>
     </row>
     <row r="25">
-      <c r="A25" s="61"/>
-      <c r="B25" s="70"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="33"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="36"/>
     </row>
     <row r="26">
-      <c r="A26" s="72"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="64"/>
+      <c r="A26" s="75"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="67"/>
     </row>
     <row r="27">
-      <c r="A27" s="61"/>
-      <c r="B27" s="70"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="33"/>
+      <c r="A27" s="64"/>
+      <c r="B27" s="73"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28">
-      <c r="A28" s="68">
+      <c r="A28" s="71">
         <f t="shared" ref="A28:B28" si="6">A11</f>
         <v>3</v>
       </c>
-      <c r="B28" s="69" t="str">
+      <c r="B28" s="72" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
     </row>
     <row r="29">
-      <c r="A29" s="61"/>
-      <c r="B29" s="70"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
+      <c r="A29" s="64"/>
+      <c r="B29" s="73"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
     </row>
     <row r="30">
-      <c r="A30" s="72"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
+      <c r="A30" s="75"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
     </row>
     <row r="31">
-      <c r="A31" s="61"/>
-      <c r="B31" s="70"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
+      <c r="A31" s="64"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
     </row>
     <row r="32">
-      <c r="A32" s="72"/>
-      <c r="B32" s="64"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
+      <c r="A32" s="75"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
     </row>
     <row r="33">
-      <c r="A33" s="61"/>
-      <c r="B33" s="70"/>
-      <c r="C33" s="73" t="s">
-        <v>147</v>
-      </c>
-      <c r="D33" s="56"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
+      <c r="A33" s="64"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="76" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="59"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34">
-      <c r="A34" s="72"/>
-      <c r="B34" s="64"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
+      <c r="A34" s="75"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>